<commit_message>
make retrieveGeneralInformation an extension function
</commit_message>
<xml_diff>
--- a/src/main/resources/simple_sheet.xlsx
+++ b/src/main/resources/simple_sheet.xlsx
@@ -3401,16 +3401,16 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3808,8 +3808,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3870,7 +3870,7 @@
         <v>Should be provided for this model class?</v>
       </c>
       <c r="J1" s="15"/>
-      <c r="K1" s="22" t="str">
+      <c r="K1" s="25" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("Importrange(""https://docs.google.com/spreadsheets/d/1R5ofJAIqAywN97cnBY9R9kqj10AvQOs3Gq472n6iDyc/edit?usp=sharing"",""Dose-response Model!C5"")"),"Creator(s)")</f>
         <v>Creator(s)</v>
       </c>
@@ -3885,7 +3885,7 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -4798,7 +4798,7 @@
       <c r="C27" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="26" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -5004,7 +5004,7 @@
       <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="22" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="24" t="s">
@@ -5869,7 +5869,7 @@
       <c r="I76" t="s">
         <v>6</v>
       </c>
-      <c r="K76" s="22" t="s">
+      <c r="K76" s="25" t="s">
         <v>30</v>
       </c>
       <c r="L76" s="23"/>
@@ -5938,7 +5938,7 @@
       <c r="A79" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="22" t="s">
         <v>115</v>
       </c>
       <c r="C79" s="24" t="s">
@@ -6903,7 +6903,7 @@
       <c r="A123" t="s">
         <v>6</v>
       </c>
-      <c r="B123" s="26" t="s">
+      <c r="B123" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C123" s="24" t="s">
@@ -7941,7 +7941,7 @@
       <c r="A158" t="s">
         <v>30</v>
       </c>
-      <c r="B158" s="26" t="s">
+      <c r="B158" s="22" t="s">
         <v>211</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -15607,45 +15607,6 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="55">
-    <mergeCell ref="B123:B157"/>
-    <mergeCell ref="B158:B163"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="C123:C140"/>
-    <mergeCell ref="C152:C156"/>
-    <mergeCell ref="C143:C150"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="C114:C122"/>
-    <mergeCell ref="C105:C110"/>
-    <mergeCell ref="B2:B36"/>
-    <mergeCell ref="C62:C74"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="C95:C104"/>
-    <mergeCell ref="C79:C94"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="B37:B78"/>
-    <mergeCell ref="B79:B122"/>
-    <mergeCell ref="C48:C61"/>
-    <mergeCell ref="C37:C47"/>
-    <mergeCell ref="D159:F159"/>
-    <mergeCell ref="D162:F162"/>
-    <mergeCell ref="D163:F163"/>
-    <mergeCell ref="D161:F161"/>
-    <mergeCell ref="D160:F160"/>
-    <mergeCell ref="D114:D122"/>
-    <mergeCell ref="D111:D113"/>
-    <mergeCell ref="D79:D94"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D158:F158"/>
-    <mergeCell ref="D123:D140"/>
-    <mergeCell ref="D152:D156"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="D143:D150"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D48:D61"/>
-    <mergeCell ref="D37:D47"/>
-    <mergeCell ref="D105:D110"/>
-    <mergeCell ref="D95:D104"/>
     <mergeCell ref="K1:Q1"/>
     <mergeCell ref="K76:L76"/>
     <mergeCell ref="D75:F75"/>
@@ -15662,6 +15623,45 @@
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D48:D61"/>
+    <mergeCell ref="D37:D47"/>
+    <mergeCell ref="D105:D110"/>
+    <mergeCell ref="D95:D104"/>
+    <mergeCell ref="D114:D122"/>
+    <mergeCell ref="D111:D113"/>
+    <mergeCell ref="D79:D94"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="D123:D140"/>
+    <mergeCell ref="D152:D156"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="D143:D150"/>
+    <mergeCell ref="D159:F159"/>
+    <mergeCell ref="D162:F162"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="D161:F161"/>
+    <mergeCell ref="D160:F160"/>
+    <mergeCell ref="C105:C110"/>
+    <mergeCell ref="B2:B36"/>
+    <mergeCell ref="C62:C74"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="C95:C104"/>
+    <mergeCell ref="C79:C94"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="B37:B78"/>
+    <mergeCell ref="B79:B122"/>
+    <mergeCell ref="C48:C61"/>
+    <mergeCell ref="C37:C47"/>
+    <mergeCell ref="B123:B157"/>
+    <mergeCell ref="B158:B163"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="C123:C140"/>
+    <mergeCell ref="C152:C156"/>
+    <mergeCell ref="C143:C150"/>
+    <mergeCell ref="C141:C142"/>
+    <mergeCell ref="C114:C122"/>
   </mergeCells>
   <dataValidations count="51">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Yes or No" sqref="H9 K14:K18">

</xml_diff>